<commit_message>
Adicionado os Arquivos de Desenvolvimento do Sistema Web
Adicionado os Arquivos de Desenvolvimento do Sistema Web e também começado o modelamento do banco de dados
</commit_message>
<xml_diff>
--- a/Diário de Bordo VolunTrab.xlsx
+++ b/Diário de Bordo VolunTrab.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Aulas do Curso\3° Ano\PTCC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VolunTrab\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="33">
   <si>
     <t xml:space="preserve">Diário de Bordo </t>
   </si>
@@ -166,6 +166,24 @@
   </si>
   <si>
     <t>Orientção sobre a parte escrita do TCC</t>
+  </si>
+  <si>
+    <t>Conselho de Classe/Semana Paulo Freire</t>
+  </si>
+  <si>
+    <t>Semana Paulo Freire</t>
+  </si>
+  <si>
+    <t>Inicio da Introdução da Parte escrita do Tcc</t>
+  </si>
+  <si>
+    <t>E continuado o desenvolvimento do Mockup</t>
+  </si>
+  <si>
+    <t>Desenvolvido a Introdução da parte escrita Tcc</t>
+  </si>
+  <si>
+    <t>Mockup no processo de finalização</t>
   </si>
 </sst>
 </file>
@@ -936,8 +954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +963,7 @@
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="10" width="5.7109375" customWidth="1"/>
     <col min="11" max="11" width="55.42578125" customWidth="1"/>
-    <col min="12" max="12" width="25.85546875" customWidth="1"/>
+    <col min="12" max="12" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1279,69 +1297,153 @@
       </c>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>42852</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="8"/>
+      <c r="B14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="L14" s="9"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>42859</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="8"/>
+      <c r="B15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>28</v>
+      </c>
       <c r="L15" s="9"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>42866</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="9"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>42873</v>
       </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="9"/>
+      <c r="B17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="6">

</xml_diff>

<commit_message>
Adicionado parte escrita Tcc, Atualizado o mockup
</commit_message>
<xml_diff>
--- a/Diário de Bordo VolunTrab.xlsx
+++ b/Diário de Bordo VolunTrab.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="37">
   <si>
     <t xml:space="preserve">Diário de Bordo </t>
   </si>
@@ -184,6 +184,18 @@
   </si>
   <si>
     <t>Mockup no processo de finalização</t>
+  </si>
+  <si>
+    <t>Termino da Introdução da parte escrita Tcc</t>
+  </si>
+  <si>
+    <t>Atualizado o Kanban</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> continuação da Aula sobre formatação ABNT no word</t>
+  </si>
+  <si>
+    <t>Reuniao de ajustes do mockup, tirado duvidas sobre a estrutura do site</t>
   </si>
 </sst>
 </file>
@@ -565,7 +577,7 @@
         <xdr:cNvPr id="2" name="Imagem 1" descr="Descrição: 2010-07_logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -618,7 +630,7 @@
         <xdr:cNvPr id="3" name="Caixa de texto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -955,7 +967,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1445,48 +1457,114 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>42880</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="9"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="8"/>
+      <c r="B18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>42887</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
-      <c r="K20" s="8"/>
+    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>42894</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K20" s="8" t="s">
+        <v>36</v>
+      </c>
       <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualização Diario de Bordo
</commit_message>
<xml_diff>
--- a/Diário de Bordo VolunTrab.xlsx
+++ b/Diário de Bordo VolunTrab.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VolunTrab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Aulas do Curso\3° Ano\3°Bimestre\TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="38">
   <si>
     <t xml:space="preserve">Diário de Bordo </t>
   </si>
@@ -165,37 +165,40 @@
     <t>Palestra com os alunos da USP</t>
   </si>
   <si>
-    <t>Orientção sobre a parte escrita do TCC</t>
-  </si>
-  <si>
-    <t>Conselho de Classe/Semana Paulo Freire</t>
+    <t>Orientação sobre a parte escrita do TCC</t>
+  </si>
+  <si>
+    <t>Reunião sobre a SPF</t>
+  </si>
+  <si>
+    <t>Conselho de Classe</t>
+  </si>
+  <si>
+    <t>Pesquisas sobre o contexto e Introdução do TCC</t>
   </si>
   <si>
     <t>Semana Paulo Freire</t>
   </si>
   <si>
-    <t>Inicio da Introdução da Parte escrita do Tcc</t>
-  </si>
-  <si>
-    <t>E continuado o desenvolvimento do Mockup</t>
-  </si>
-  <si>
-    <t>Desenvolvido a Introdução da parte escrita Tcc</t>
-  </si>
-  <si>
-    <t>Mockup no processo de finalização</t>
-  </si>
-  <si>
-    <t>Termino da Introdução da parte escrita Tcc</t>
-  </si>
-  <si>
-    <t>Atualizado o Kanban</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> continuação da Aula sobre formatação ABNT no word</t>
-  </si>
-  <si>
-    <t>Reuniao de ajustes do mockup, tirado duvidas sobre a estrutura do site</t>
+    <t xml:space="preserve">Introdução do TCC </t>
+  </si>
+  <si>
+    <t>Entrega do TCC-primeira parte</t>
+  </si>
+  <si>
+    <t>avaliação dos TCCs</t>
+  </si>
+  <si>
+    <t>Feriado Corpus Christi</t>
+  </si>
+  <si>
+    <t>Revisão da primeira parte do TCC</t>
+  </si>
+  <si>
+    <t>Revisão do TCC, Modelagem do BD, Elaboração de uma carta para enviar para as instituições.</t>
+  </si>
+  <si>
+    <t>Finalização do BD, Metodologia da escrita do TCC, Árvore (design)</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -494,6 +497,10 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -577,7 +584,7 @@
         <xdr:cNvPr id="2" name="Imagem 1" descr="Descrição: 2010-07_logo">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -630,7 +637,7 @@
         <xdr:cNvPr id="3" name="Caixa de texto 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -967,7 +974,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -975,24 +982,24 @@
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="10" width="5.7109375" customWidth="1"/>
     <col min="11" max="11" width="55.42578125" customWidth="1"/>
-    <col min="12" max="12" width="40.42578125" customWidth="1"/>
+    <col min="12" max="12" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="16"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="17"/>
     </row>
     <row r="2" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -1012,18 +1019,18 @@
       <c r="A3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
       <c r="L3" s="13" t="s">
         <v>8</v>
       </c>
@@ -1032,19 +1039,19 @@
       <c r="A4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="26"/>
     </row>
     <row r="5" spans="1:12" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
@@ -1064,30 +1071,30 @@
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="22"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
-      <c r="J7" s="22"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
     </row>
     <row r="8" spans="1:12" ht="231" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1309,75 +1316,41 @@
       </c>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>42852</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
       <c r="K14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="L14" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>42859</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
       <c r="K15" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L15" s="9"/>
     </row>
@@ -1409,15 +1382,11 @@
       <c r="I16" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="7" t="s">
-        <v>18</v>
-      </c>
+      <c r="J16" s="7"/>
       <c r="K16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L16" s="9" t="s">
-        <v>30</v>
-      </c>
+      <c r="L16" s="9"/>
     </row>
     <row r="17" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
@@ -1453,9 +1422,7 @@
       <c r="K17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="L17" s="9" t="s">
-        <v>32</v>
-      </c>
+      <c r="L17" s="9"/>
     </row>
     <row r="18" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
@@ -1489,11 +1456,9 @@
         <v>18</v>
       </c>
       <c r="K18" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="L18" s="9" t="s">
-        <v>34</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="L18" s="9"/>
     </row>
     <row r="19" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
@@ -1527,11 +1492,11 @@
         <v>18</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L19" s="9"/>
     </row>
-    <row r="20" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>42894</v>
       </c>
@@ -1563,12 +1528,14 @@
         <v>18</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L20" s="9"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="A21" s="6">
+        <v>42901</v>
+      </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -1578,11 +1545,15 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
-      <c r="K21" s="8"/>
+      <c r="K21" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="L21" s="9"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="A22" s="6">
+        <v>42908</v>
+      </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1595,50 +1566,110 @@
       <c r="K22" s="8"/>
       <c r="L22" s="9"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="7"/>
+    <row r="23" spans="1:12" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>42943</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="8"/>
+      <c r="D23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>35</v>
+      </c>
       <c r="L23" s="9"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="7"/>
+    <row r="24" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>42950</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="9"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="D24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K24" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="L24" s="14"/>
+    </row>
+    <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>42957</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>18</v>
+      </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="8"/>
+      <c r="J25" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K25" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="L25" s="9"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="6">
+        <v>42964</v>
+      </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -1652,7 +1683,9 @@
       <c r="L26" s="9"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+      <c r="A27" s="6">
+        <v>42971</v>
+      </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -1666,7 +1699,9 @@
       <c r="L27" s="9"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="6">
+        <v>42978</v>
+      </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -1680,7 +1715,9 @@
       <c r="L28" s="9"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
+      <c r="A29" s="6">
+        <v>42995</v>
+      </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -1694,7 +1731,9 @@
       <c r="L29" s="9"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+      <c r="A30" s="6">
+        <v>42999</v>
+      </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -1708,7 +1747,9 @@
       <c r="L30" s="9"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
+      <c r="A31" s="6">
+        <v>43006</v>
+      </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>

</xml_diff>